<commit_message>
feat: code vhdl in ROM
</commit_message>
<xml_diff>
--- a/Rendu_3/MemoryMap.xlsx
+++ b/Rendu_3/MemoryMap.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -204,16 +204,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -232,6 +232,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -500,7 +504,7 @@
   <dimension ref="B2:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,10 +513,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="30" x14ac:dyDescent="0.5">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
@@ -548,7 +552,7 @@
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -562,7 +566,7 @@
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="7" t="s">
         <v>0</v>
       </c>
     </row>
@@ -570,7 +574,7 @@
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>